<commit_message>
organización capitulos, comienzo capitulo 2
</commit_message>
<xml_diff>
--- a/agregado/resultados/1950_2000_top5_x_yr_expo.xlsx
+++ b/agregado/resultados/1950_2000_top5_x_yr_expo.xlsx
@@ -6799,7 +6799,7 @@
         <v>117</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="AB2" t="s">
         <v>113</v>
@@ -6847,7 +6847,7 @@
         <v>117</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AR2" t="s">
         <v>113</v>
@@ -6961,7 +6961,7 @@
         <v>117</v>
       </c>
       <c r="CC2" t="n">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="CD2" t="s">
         <v>112</v>
@@ -6991,7 +6991,7 @@
         <v>117</v>
       </c>
       <c r="CM2" t="n">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="CN2" t="s">
         <v>117</v>
@@ -7015,7 +7015,7 @@
         <v>112</v>
       </c>
       <c r="CU2" t="n">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="CV2" t="s">
         <v>112</v>
@@ -7033,13 +7033,13 @@
         <v>112</v>
       </c>
       <c r="DA2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>112</v>
+      </c>
+      <c r="DC2" t="n">
         <v>0.9999999999999999</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>112</v>
-      </c>
-      <c r="DC2" t="n">
-        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -7050,145 +7050,145 @@
         <v>112</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9353071644926834</v>
+        <v>0.9353071644926831</v>
       </c>
       <c r="D3" t="s">
         <v>116</v>
       </c>
       <c r="E3" t="n">
-        <v>0.962782843707968</v>
+        <v>0.9627828437079674</v>
       </c>
       <c r="F3" t="s">
         <v>112</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9695852627666819</v>
+        <v>0.9695852627666812</v>
       </c>
       <c r="H3" t="s">
         <v>116</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9465873519030232</v>
+        <v>0.9465873519030233</v>
       </c>
       <c r="J3" t="s">
         <v>113</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9968425349073488</v>
+        <v>0.9968425349073495</v>
       </c>
       <c r="L3" t="s">
         <v>117</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9997225841868417</v>
+        <v>0.999722584186841</v>
       </c>
       <c r="N3" t="s">
         <v>113</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9738363091940068</v>
+        <v>0.9738363091940054</v>
       </c>
       <c r="P3" t="s">
         <v>113</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9490910335271661</v>
+        <v>0.9490910335271655</v>
       </c>
       <c r="R3" t="s">
         <v>113</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9534594447881103</v>
+        <v>0.9534594447881102</v>
       </c>
       <c r="T3" t="s">
         <v>113</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9628056235710425</v>
+        <v>0.9628056235710422</v>
       </c>
       <c r="V3" t="s">
         <v>113</v>
       </c>
       <c r="W3" t="n">
-        <v>0.9811556033626555</v>
+        <v>0.9811556033626566</v>
       </c>
       <c r="X3" t="s">
         <v>113</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.9917484702155919</v>
+        <v>0.9917484702155904</v>
       </c>
       <c r="Z3" t="s">
         <v>113</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.9766423994891014</v>
+        <v>0.9766423994891011</v>
       </c>
       <c r="AB3" t="s">
         <v>117</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.9725441134386383</v>
+        <v>0.9725441134386372</v>
       </c>
       <c r="AD3" t="s">
         <v>113</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.9980909817901024</v>
+        <v>0.9980909817901034</v>
       </c>
       <c r="AF3" t="s">
         <v>117</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.9958349083140333</v>
+        <v>0.9958349083140335</v>
       </c>
       <c r="AH3" t="s">
         <v>117</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.9934441089557838</v>
+        <v>0.9934441089557832</v>
       </c>
       <c r="AJ3" t="s">
         <v>117</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.9857407767081481</v>
+        <v>0.9857407767081469</v>
       </c>
       <c r="AL3" t="s">
         <v>117</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.9970009902254855</v>
+        <v>0.9970009902254853</v>
       </c>
       <c r="AN3" t="s">
         <v>117</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.9899097038415406</v>
+        <v>0.9899097038415405</v>
       </c>
       <c r="AP3" t="s">
         <v>113</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.9797898763966965</v>
+        <v>0.9797898763966967</v>
       </c>
       <c r="AR3" t="s">
         <v>117</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.9834182101100295</v>
+        <v>0.9834182101100291</v>
       </c>
       <c r="AT3" t="s">
         <v>113</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.9986433343592077</v>
+        <v>0.9986433343592069</v>
       </c>
       <c r="AV3" t="s">
         <v>113</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.9848828406989165</v>
+        <v>0.9848828406989181</v>
       </c>
       <c r="AX3" t="s">
         <v>113</v>
@@ -7200,169 +7200,169 @@
         <v>113</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.9821268597846274</v>
+        <v>0.9821268597846277</v>
       </c>
       <c r="BB3" t="s">
         <v>113</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.9676824800307634</v>
+        <v>0.9676824800307645</v>
       </c>
       <c r="BD3" t="s">
         <v>113</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.9586968858751983</v>
+        <v>0.9586968858751966</v>
       </c>
       <c r="BF3" t="s">
         <v>112</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.9496473132640489</v>
+        <v>0.9496473132640483</v>
       </c>
       <c r="BH3" t="s">
         <v>113</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.9689155308151783</v>
+        <v>0.968915530815179</v>
       </c>
       <c r="BJ3" t="s">
         <v>117</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.9993383591186045</v>
+        <v>0.9993383591186041</v>
       </c>
       <c r="BL3" t="s">
         <v>117</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.9893928669950524</v>
+        <v>0.9893928669950515</v>
       </c>
       <c r="BN3" t="s">
         <v>113</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.9858455232418818</v>
+        <v>0.9858455232418833</v>
       </c>
       <c r="BP3" t="s">
         <v>112</v>
       </c>
       <c r="BQ3" t="n">
-        <v>0.9650371904639572</v>
+        <v>0.9650371904639581</v>
       </c>
       <c r="BR3" t="s">
         <v>112</v>
       </c>
       <c r="BS3" t="n">
-        <v>0.974255744986734</v>
+        <v>0.9742557449867337</v>
       </c>
       <c r="BT3" t="s">
         <v>112</v>
       </c>
       <c r="BU3" t="n">
-        <v>0.9878178306714998</v>
+        <v>0.9878178306715002</v>
       </c>
       <c r="BV3" t="s">
         <v>112</v>
       </c>
       <c r="BW3" t="n">
-        <v>0.9996015893047362</v>
+        <v>0.9996015893047371</v>
       </c>
       <c r="BX3" t="s">
         <v>112</v>
       </c>
       <c r="BY3" t="n">
-        <v>0.9607669099378496</v>
+        <v>0.9607669099378483</v>
       </c>
       <c r="BZ3" t="s">
         <v>112</v>
       </c>
       <c r="CA3" t="n">
-        <v>0.9830131040636073</v>
+        <v>0.9830131040636064</v>
       </c>
       <c r="CB3" t="s">
         <v>113</v>
       </c>
       <c r="CC3" t="n">
-        <v>0.9928550556744634</v>
+        <v>0.9928550556744646</v>
       </c>
       <c r="CD3" t="s">
         <v>113</v>
       </c>
       <c r="CE3" t="n">
-        <v>0.9979107461601509</v>
+        <v>0.9979107461601507</v>
       </c>
       <c r="CF3" t="s">
         <v>113</v>
       </c>
       <c r="CG3" t="n">
-        <v>0.9769231238045252</v>
+        <v>0.9769231238045265</v>
       </c>
       <c r="CH3" t="s">
         <v>113</v>
       </c>
       <c r="CI3" t="n">
-        <v>0.9934316346907267</v>
+        <v>0.9934316346907283</v>
       </c>
       <c r="CJ3" t="s">
         <v>117</v>
       </c>
       <c r="CK3" t="n">
-        <v>0.972792875348479</v>
+        <v>0.9727928753484785</v>
       </c>
       <c r="CL3" t="s">
         <v>112</v>
       </c>
       <c r="CM3" t="n">
-        <v>0.9977477511199129</v>
+        <v>0.9977477511199144</v>
       </c>
       <c r="CN3" t="s">
         <v>112</v>
       </c>
       <c r="CO3" t="n">
-        <v>0.9974367615403189</v>
+        <v>0.9974367615403193</v>
       </c>
       <c r="CP3" t="s">
         <v>117</v>
       </c>
       <c r="CQ3" t="n">
-        <v>0.9925564055523348</v>
+        <v>0.9925564055523346</v>
       </c>
       <c r="CR3" t="s">
         <v>117</v>
       </c>
       <c r="CS3" t="n">
-        <v>0.9978238260296356</v>
+        <v>0.9978238260296352</v>
       </c>
       <c r="CT3" t="s">
         <v>117</v>
       </c>
       <c r="CU3" t="n">
-        <v>0.993874328683789</v>
+        <v>0.9938743286837912</v>
       </c>
       <c r="CV3" t="s">
         <v>117</v>
       </c>
       <c r="CW3" t="n">
-        <v>0.9901939825818409</v>
+        <v>0.99019398258184</v>
       </c>
       <c r="CX3" t="s">
         <v>117</v>
       </c>
       <c r="CY3" t="n">
-        <v>0.9916546225773024</v>
+        <v>0.9916546225773005</v>
       </c>
       <c r="CZ3" t="s">
         <v>117</v>
       </c>
       <c r="DA3" t="n">
-        <v>0.9680382301380499</v>
+        <v>0.9680382301380522</v>
       </c>
       <c r="DB3" t="s">
         <v>117</v>
       </c>
       <c r="DC3" t="n">
-        <v>0.9593966523950025</v>
+        <v>0.9593966523950017</v>
       </c>
     </row>
     <row r="4">
@@ -7373,319 +7373,319 @@
         <v>116</v>
       </c>
       <c r="C4" t="n">
-        <v>0.918329395219955</v>
+        <v>0.9183293952199553</v>
       </c>
       <c r="D4" t="s">
         <v>112</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9535709286123478</v>
+        <v>0.9535709286123482</v>
       </c>
       <c r="F4" t="s">
         <v>116</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9264681971802706</v>
+        <v>0.9264681971802704</v>
       </c>
       <c r="H4" t="s">
         <v>117</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9461938460967997</v>
+        <v>0.9461938460968005</v>
       </c>
       <c r="J4" t="s">
         <v>112</v>
       </c>
       <c r="K4" t="n">
-        <v>0.963608369975863</v>
+        <v>0.9636083699758631</v>
       </c>
       <c r="L4" t="s">
         <v>112</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9631686475765593</v>
+        <v>0.9631686475765591</v>
       </c>
       <c r="N4" t="s">
         <v>112</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9297410724376485</v>
+        <v>0.9297410724376488</v>
       </c>
       <c r="P4" t="s">
         <v>112</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9356957441390211</v>
+        <v>0.9356957441390208</v>
       </c>
       <c r="R4" t="s">
         <v>112</v>
       </c>
       <c r="S4" t="n">
-        <v>0.9087999893058523</v>
+        <v>0.9087999893058535</v>
       </c>
       <c r="T4" t="s">
         <v>112</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9407897732093299</v>
+        <v>0.9407897732093291</v>
       </c>
       <c r="V4" t="s">
         <v>112</v>
       </c>
       <c r="W4" t="n">
-        <v>0.9339981375340533</v>
+        <v>0.933998137534053</v>
       </c>
       <c r="X4" t="s">
         <v>112</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.9380006870621875</v>
+        <v>0.938000687062188</v>
       </c>
       <c r="Z4" t="s">
         <v>116</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.9218658977627006</v>
+        <v>0.9218658977626991</v>
       </c>
       <c r="AB4" t="s">
         <v>112</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.9257224056703104</v>
+        <v>0.9257224056703108</v>
       </c>
       <c r="AD4" t="s">
         <v>112</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.9512402755519891</v>
+        <v>0.9512402755519895</v>
       </c>
       <c r="AF4" t="s">
         <v>116</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.9320546365281038</v>
+        <v>0.9320546365281036</v>
       </c>
       <c r="AH4" t="s">
         <v>112</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.9376767260788718</v>
+        <v>0.9376767260788708</v>
       </c>
       <c r="AJ4" t="s">
         <v>112</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.9370174842685455</v>
+        <v>0.9370174842685465</v>
       </c>
       <c r="AL4" t="s">
         <v>112</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.9225254598913595</v>
+        <v>0.9225254598913583</v>
       </c>
       <c r="AN4" t="s">
         <v>116</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.9159405779092236</v>
+        <v>0.9159405779092242</v>
       </c>
       <c r="AP4" t="s">
         <v>112</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.8910111999157769</v>
+        <v>0.891011199915776</v>
       </c>
       <c r="AR4" t="s">
         <v>112</v>
       </c>
       <c r="AS4" t="n">
-        <v>0.9048501163806192</v>
+        <v>0.9048501163806199</v>
       </c>
       <c r="AT4" t="s">
         <v>112</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.9098537189150445</v>
+        <v>0.9098537189150454</v>
       </c>
       <c r="AV4" t="s">
         <v>112</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.919449733408543</v>
+        <v>0.9194497334085441</v>
       </c>
       <c r="AX4" t="s">
         <v>112</v>
       </c>
       <c r="AY4" t="n">
-        <v>0.9410941777104936</v>
+        <v>0.9410941777104922</v>
       </c>
       <c r="AZ4" t="s">
         <v>112</v>
       </c>
       <c r="BA4" t="n">
-        <v>0.9464933571353829</v>
+        <v>0.9464933571353831</v>
       </c>
       <c r="BB4" t="s">
         <v>116</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.9586463931823626</v>
+        <v>0.9586463931823618</v>
       </c>
       <c r="BD4" t="s">
         <v>112</v>
       </c>
       <c r="BE4" t="n">
-        <v>0.9108892446112162</v>
+        <v>0.9108892446112146</v>
       </c>
       <c r="BF4" t="s">
         <v>113</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.9487747627962472</v>
+        <v>0.9487747627962465</v>
       </c>
       <c r="BH4" t="s">
         <v>112</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.9684201947376078</v>
+        <v>0.9684201947376087</v>
       </c>
       <c r="BJ4" t="s">
         <v>113</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.9861359422231986</v>
+        <v>0.9861359422231984</v>
       </c>
       <c r="BL4" t="s">
         <v>113</v>
       </c>
       <c r="BM4" t="n">
-        <v>0.9799348255982141</v>
+        <v>0.9799348255982151</v>
       </c>
       <c r="BN4" t="s">
         <v>112</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.9852136094290008</v>
+        <v>0.9852136094290013</v>
       </c>
       <c r="BP4" t="s">
         <v>115</v>
       </c>
       <c r="BQ4" t="n">
-        <v>0.9627691324217156</v>
+        <v>0.9627691324217171</v>
       </c>
       <c r="BR4" t="s">
         <v>113</v>
       </c>
       <c r="BS4" t="n">
-        <v>0.9615385446269882</v>
+        <v>0.9615385446269874</v>
       </c>
       <c r="BT4" t="s">
         <v>113</v>
       </c>
       <c r="BU4" t="n">
-        <v>0.949718522266766</v>
+        <v>0.9497185222667667</v>
       </c>
       <c r="BV4" t="s">
         <v>113</v>
       </c>
       <c r="BW4" t="n">
-        <v>0.9725070637076791</v>
+        <v>0.9725070637076798</v>
       </c>
       <c r="BX4" t="s">
         <v>113</v>
       </c>
       <c r="BY4" t="n">
-        <v>0.94223907356856</v>
+        <v>0.9422390735685597</v>
       </c>
       <c r="BZ4" t="s">
         <v>113</v>
       </c>
       <c r="CA4" t="n">
-        <v>0.978879912865644</v>
+        <v>0.9788799128656432</v>
       </c>
       <c r="CB4" t="s">
         <v>112</v>
       </c>
       <c r="CC4" t="n">
-        <v>0.9850731970384882</v>
+        <v>0.9850731970384885</v>
       </c>
       <c r="CD4" t="s">
         <v>117</v>
       </c>
       <c r="CE4" t="n">
-        <v>0.9963212275086689</v>
+        <v>0.9963212275086694</v>
       </c>
       <c r="CF4" t="s">
         <v>117</v>
       </c>
       <c r="CG4" t="n">
-        <v>0.9691167807971903</v>
+        <v>0.9691167807971921</v>
       </c>
       <c r="CH4" t="s">
         <v>117</v>
       </c>
       <c r="CI4" t="n">
-        <v>0.9694574822616111</v>
+        <v>0.9694574822616124</v>
       </c>
       <c r="CJ4" t="s">
         <v>116</v>
       </c>
       <c r="CK4" t="n">
-        <v>0.9439157268595746</v>
+        <v>0.9439157268595758</v>
       </c>
       <c r="CL4" t="s">
         <v>116</v>
       </c>
       <c r="CM4" t="n">
-        <v>0.9448567038863661</v>
+        <v>0.9448567038863673</v>
       </c>
       <c r="CN4" t="s">
         <v>113</v>
       </c>
       <c r="CO4" t="n">
-        <v>0.9493100145710603</v>
+        <v>0.9493100145710612</v>
       </c>
       <c r="CP4" t="s">
         <v>113</v>
       </c>
       <c r="CQ4" t="n">
-        <v>0.9718995204486399</v>
+        <v>0.9718995204486379</v>
       </c>
       <c r="CR4" t="s">
         <v>113</v>
       </c>
       <c r="CS4" t="n">
-        <v>0.9581223584195928</v>
+        <v>0.9581223584195921</v>
       </c>
       <c r="CT4" t="s">
         <v>113</v>
       </c>
       <c r="CU4" t="n">
-        <v>0.9561593664781591</v>
+        <v>0.9561593664781599</v>
       </c>
       <c r="CV4" t="s">
         <v>113</v>
       </c>
       <c r="CW4" t="n">
-        <v>0.945185308626906</v>
+        <v>0.9451853086269052</v>
       </c>
       <c r="CX4" t="s">
         <v>113</v>
       </c>
       <c r="CY4" t="n">
-        <v>0.940012343059542</v>
+        <v>0.9400123430595417</v>
       </c>
       <c r="CZ4" t="s">
         <v>113</v>
       </c>
       <c r="DA4" t="n">
-        <v>0.9482652247943602</v>
+        <v>0.9482652247943613</v>
       </c>
       <c r="DB4" t="s">
         <v>113</v>
       </c>
       <c r="DC4" t="n">
-        <v>0.9288689964792902</v>
+        <v>0.9288689964792904</v>
       </c>
     </row>
     <row r="5">
@@ -7702,7 +7702,7 @@
         <v>115</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9399462228061902</v>
+        <v>0.9399462228061888</v>
       </c>
       <c r="F5" t="s">
         <v>117</v>
@@ -7714,103 +7714,103 @@
         <v>112</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9399516318463803</v>
+        <v>0.9399516318463804</v>
       </c>
       <c r="J5" t="s">
         <v>117</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9595370631954773</v>
+        <v>0.9595370631954772</v>
       </c>
       <c r="L5" t="s">
         <v>115</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9350121080740094</v>
+        <v>0.9350121080740087</v>
       </c>
       <c r="N5" t="s">
         <v>116</v>
       </c>
       <c r="O5" t="n">
-        <v>0.9198753332165599</v>
+        <v>0.9198753332165602</v>
       </c>
       <c r="P5" t="s">
         <v>115</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.9147464546076981</v>
+        <v>0.914746454607697</v>
       </c>
       <c r="R5" t="s">
         <v>116</v>
       </c>
       <c r="S5" t="n">
-        <v>0.8870477198795803</v>
+        <v>0.8870477198795805</v>
       </c>
       <c r="T5" t="s">
         <v>115</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9187512082338265</v>
+        <v>0.9187512082338258</v>
       </c>
       <c r="V5" t="s">
         <v>116</v>
       </c>
       <c r="W5" t="n">
-        <v>0.9094005229930665</v>
+        <v>0.909400522993068</v>
       </c>
       <c r="X5" t="s">
         <v>116</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.8693753604339325</v>
+        <v>0.8693753604339315</v>
       </c>
       <c r="Z5" t="s">
         <v>112</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.9125075375922559</v>
+        <v>0.9125075375922558</v>
       </c>
       <c r="AB5" t="s">
         <v>116</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.8954744278830408</v>
+        <v>0.8954744278830404</v>
       </c>
       <c r="AD5" t="s">
         <v>116</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.9093526694646171</v>
+        <v>0.9093526694646176</v>
       </c>
       <c r="AF5" t="s">
         <v>112</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.9291085956502685</v>
+        <v>0.9291085956502669</v>
       </c>
       <c r="AH5" t="s">
         <v>116</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.9090383892106791</v>
+        <v>0.9090383892106787</v>
       </c>
       <c r="AJ5" t="s">
         <v>116</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.9102192097799933</v>
+        <v>0.9102192097799942</v>
       </c>
       <c r="AL5" t="s">
         <v>116</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.921113999804989</v>
+        <v>0.9211139998049882</v>
       </c>
       <c r="AN5" t="s">
         <v>112</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.9156794489430403</v>
+        <v>0.9156794489430408</v>
       </c>
       <c r="AP5" t="s">
         <v>116</v>
@@ -7822,187 +7822,187 @@
         <v>116</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.8940785756973063</v>
+        <v>0.8940785756973061</v>
       </c>
       <c r="AT5" t="s">
         <v>116</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.8946245893889273</v>
+        <v>0.8946245893889258</v>
       </c>
       <c r="AV5" t="s">
         <v>116</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.9024291064292789</v>
+        <v>0.90242910642928</v>
       </c>
       <c r="AX5" t="s">
         <v>116</v>
       </c>
       <c r="AY5" t="n">
-        <v>0.9104535173539677</v>
+        <v>0.9104535173539668</v>
       </c>
       <c r="AZ5" t="s">
         <v>116</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.9105219746003903</v>
+        <v>0.9105219746003906</v>
       </c>
       <c r="BB5" t="s">
         <v>112</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.9285441519329874</v>
+        <v>0.9285441519329863</v>
       </c>
       <c r="BD5" t="s">
         <v>116</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.8879361218521509</v>
+        <v>0.8879361218521498</v>
       </c>
       <c r="BF5" t="s">
         <v>116</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.8836933178212892</v>
+        <v>0.8836933178212886</v>
       </c>
       <c r="BH5" t="s">
         <v>116</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.8968546962980575</v>
+        <v>0.8968546962980578</v>
       </c>
       <c r="BJ5" t="s">
         <v>115</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.9086614372354018</v>
+        <v>0.908661437235401</v>
       </c>
       <c r="BL5" t="s">
         <v>116</v>
       </c>
       <c r="BM5" t="n">
-        <v>0.9291411612241677</v>
+        <v>0.9291411612241668</v>
       </c>
       <c r="BN5" t="s">
         <v>116</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.9666876683915797</v>
+        <v>0.9666876683915787</v>
       </c>
       <c r="BP5" t="s">
         <v>113</v>
       </c>
       <c r="BQ5" t="n">
-        <v>0.9515913853234834</v>
+        <v>0.951591385323485</v>
       </c>
       <c r="BR5" t="s">
         <v>115</v>
       </c>
       <c r="BS5" t="n">
-        <v>0.9481709063201786</v>
+        <v>0.9481709063201792</v>
       </c>
       <c r="BT5" t="s">
         <v>115</v>
       </c>
       <c r="BU5" t="n">
-        <v>0.9402227838864384</v>
+        <v>0.9402227838864379</v>
       </c>
       <c r="BV5" t="s">
         <v>116</v>
       </c>
       <c r="BW5" t="n">
-        <v>0.9134660758905536</v>
+        <v>0.9134660758905527</v>
       </c>
       <c r="BX5" t="s">
         <v>115</v>
       </c>
       <c r="BY5" t="n">
-        <v>0.9219113778934247</v>
+        <v>0.921911377893425</v>
       </c>
       <c r="BZ5" t="s">
         <v>115</v>
       </c>
       <c r="CA5" t="n">
-        <v>0.9520503930172309</v>
+        <v>0.9520503930172304</v>
       </c>
       <c r="CB5" t="s">
         <v>115</v>
       </c>
       <c r="CC5" t="n">
-        <v>0.9568788907565186</v>
+        <v>0.9568788907565196</v>
       </c>
       <c r="CD5" t="s">
         <v>116</v>
       </c>
       <c r="CE5" t="n">
-        <v>0.9810681980792552</v>
+        <v>0.9810681980792553</v>
       </c>
       <c r="CF5" t="s">
         <v>116</v>
       </c>
       <c r="CG5" t="n">
-        <v>0.9510997681651817</v>
+        <v>0.9510997681651818</v>
       </c>
       <c r="CH5" t="s">
         <v>116</v>
       </c>
       <c r="CI5" t="n">
-        <v>0.9636898083646916</v>
+        <v>0.9636898083646924</v>
       </c>
       <c r="CJ5" t="s">
         <v>115</v>
       </c>
       <c r="CK5" t="n">
-        <v>0.9309631058726369</v>
+        <v>0.9309631058726366</v>
       </c>
       <c r="CL5" t="s">
         <v>113</v>
       </c>
       <c r="CM5" t="n">
-        <v>0.9305581683581172</v>
+        <v>0.9305581683581184</v>
       </c>
       <c r="CN5" t="s">
         <v>115</v>
       </c>
       <c r="CO5" t="n">
-        <v>0.9235938397251623</v>
+        <v>0.9235938397251632</v>
       </c>
       <c r="CP5" t="s">
         <v>115</v>
       </c>
       <c r="CQ5" t="n">
-        <v>0.9017446043144496</v>
+        <v>0.9017446043144486</v>
       </c>
       <c r="CR5" t="s">
         <v>115</v>
       </c>
       <c r="CS5" t="n">
-        <v>0.9098386101570138</v>
+        <v>0.9098386101570127</v>
       </c>
       <c r="CT5" t="s">
         <v>116</v>
       </c>
       <c r="CU5" t="n">
-        <v>0.896174205593493</v>
+        <v>0.8961742055934938</v>
       </c>
       <c r="CV5" t="s">
         <v>115</v>
       </c>
       <c r="CW5" t="n">
-        <v>0.8912610786890895</v>
+        <v>0.8912610786890888</v>
       </c>
       <c r="CX5" t="s">
         <v>115</v>
       </c>
       <c r="CY5" t="n">
-        <v>0.9094725154650838</v>
+        <v>0.9094725154650835</v>
       </c>
       <c r="CZ5" t="s">
         <v>115</v>
       </c>
       <c r="DA5" t="n">
-        <v>0.9169229424046921</v>
+        <v>0.916922942404694</v>
       </c>
       <c r="DB5" t="s">
         <v>116</v>
@@ -8019,211 +8019,211 @@
         <v>115</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8944064831766663</v>
+        <v>0.8944064831766668</v>
       </c>
       <c r="D6" t="s">
         <v>114</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9217009271384273</v>
+        <v>0.9217009271384262</v>
       </c>
       <c r="F6" t="s">
         <v>114</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9002651166602325</v>
+        <v>0.9002651166602321</v>
       </c>
       <c r="H6" t="s">
         <v>115</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9309741078744932</v>
+        <v>0.9309741078744933</v>
       </c>
       <c r="J6" t="s">
         <v>115</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9429952141977953</v>
+        <v>0.9429952141977963</v>
       </c>
       <c r="L6" t="s">
         <v>116</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9235402394505519</v>
+        <v>0.9235402394505502</v>
       </c>
       <c r="N6" t="s">
         <v>114</v>
       </c>
       <c r="O6" t="n">
-        <v>0.9012065474348089</v>
+        <v>0.901206547434809</v>
       </c>
       <c r="P6" t="s">
         <v>116</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.8624881332988327</v>
+        <v>0.8624881332988323</v>
       </c>
       <c r="R6" t="s">
         <v>115</v>
       </c>
       <c r="S6" t="n">
-        <v>0.855318436366186</v>
+        <v>0.855318436366187</v>
       </c>
       <c r="T6" t="s">
         <v>116</v>
       </c>
       <c r="U6" t="n">
-        <v>0.8947501365552388</v>
+        <v>0.8947501365552368</v>
       </c>
       <c r="V6" t="s">
         <v>115</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8937327748944756</v>
+        <v>0.8937327748944752</v>
       </c>
       <c r="X6" t="s">
         <v>114</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.8275197451826551</v>
+        <v>0.8275197451826548</v>
       </c>
       <c r="Z6" t="s">
         <v>115</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.864891093579401</v>
+        <v>0.8648910935793996</v>
       </c>
       <c r="AB6" t="s">
         <v>115</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.8392236159802177</v>
+        <v>0.839223615980218</v>
       </c>
       <c r="AD6" t="s">
         <v>115</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.8620305264067425</v>
+        <v>0.8620305264067423</v>
       </c>
       <c r="AF6" t="s">
         <v>115</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.8476036773268413</v>
+        <v>0.8476036773268415</v>
       </c>
       <c r="AH6" t="s">
         <v>115</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.8598369321863202</v>
+        <v>0.8598369321863195</v>
       </c>
       <c r="AJ6" t="s">
         <v>115</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.8437034209178697</v>
+        <v>0.84370342091787</v>
       </c>
       <c r="AL6" t="s">
         <v>114</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.8238319465947672</v>
+        <v>0.8238319465947661</v>
       </c>
       <c r="AN6" t="s">
         <v>115</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.8474068548923551</v>
+        <v>0.8474068548923555</v>
       </c>
       <c r="AP6" t="s">
         <v>114</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.8246940936387567</v>
+        <v>0.8246940936387563</v>
       </c>
       <c r="AR6" t="s">
         <v>115</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.8480887770943395</v>
+        <v>0.8480887770943389</v>
       </c>
       <c r="AT6" t="s">
         <v>115</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.8246435013280291</v>
+        <v>0.8246435013280295</v>
       </c>
       <c r="AV6" t="s">
         <v>115</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.8324847720634385</v>
+        <v>0.8324847720634388</v>
       </c>
       <c r="AX6" t="s">
         <v>115</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.8462270652750271</v>
+        <v>0.8462270652750264</v>
       </c>
       <c r="AZ6" t="s">
         <v>114</v>
       </c>
       <c r="BA6" t="n">
-        <v>0.8572964292601937</v>
+        <v>0.8572964292601936</v>
       </c>
       <c r="BB6" t="s">
         <v>115</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.8507115519249191</v>
+        <v>0.850711551924918</v>
       </c>
       <c r="BD6" t="s">
         <v>114</v>
       </c>
       <c r="BE6" t="n">
-        <v>0.8256659345684515</v>
+        <v>0.825665934568451</v>
       </c>
       <c r="BF6" t="s">
         <v>115</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.8695714945726584</v>
+        <v>0.8695714945726577</v>
       </c>
       <c r="BH6" t="s">
         <v>115</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.8862904730645096</v>
+        <v>0.8862904730645103</v>
       </c>
       <c r="BJ6" t="s">
         <v>114</v>
       </c>
       <c r="BK6" t="n">
-        <v>0.9052933432593313</v>
+        <v>0.9052933432593302</v>
       </c>
       <c r="BL6" t="s">
         <v>115</v>
       </c>
       <c r="BM6" t="n">
-        <v>0.9147877371695032</v>
+        <v>0.9147877371695026</v>
       </c>
       <c r="BN6" t="s">
         <v>115</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.9641301789681305</v>
+        <v>0.9641301789681309</v>
       </c>
       <c r="BP6" t="s">
         <v>116</v>
       </c>
       <c r="BQ6" t="n">
-        <v>0.8909046651381719</v>
+        <v>0.8909046651381728</v>
       </c>
       <c r="BR6" t="s">
         <v>116</v>
       </c>
       <c r="BS6" t="n">
-        <v>0.8948614343523462</v>
+        <v>0.8948614343523458</v>
       </c>
       <c r="BT6" t="s">
         <v>116</v>
@@ -8235,13 +8235,13 @@
         <v>115</v>
       </c>
       <c r="BW6" t="n">
-        <v>0.9022565153515654</v>
+        <v>0.9022565153515651</v>
       </c>
       <c r="BX6" t="s">
         <v>116</v>
       </c>
       <c r="BY6" t="n">
-        <v>0.912728386090156</v>
+        <v>0.9127283860901554</v>
       </c>
       <c r="BZ6" t="s">
         <v>116</v>
@@ -8253,85 +8253,85 @@
         <v>116</v>
       </c>
       <c r="CC6" t="n">
-        <v>0.9373592384307459</v>
+        <v>0.9373592384307456</v>
       </c>
       <c r="CD6" t="s">
         <v>115</v>
       </c>
       <c r="CE6" t="n">
-        <v>0.9669069630229321</v>
+        <v>0.9669069630229318</v>
       </c>
       <c r="CF6" t="s">
         <v>115</v>
       </c>
       <c r="CG6" t="n">
-        <v>0.9433377151000961</v>
+        <v>0.9433377151000966</v>
       </c>
       <c r="CH6" t="s">
         <v>115</v>
       </c>
       <c r="CI6" t="n">
-        <v>0.9438018629326796</v>
+        <v>0.9438018629326802</v>
       </c>
       <c r="CJ6" t="s">
         <v>113</v>
       </c>
       <c r="CK6" t="n">
-        <v>0.9308451893989939</v>
+        <v>0.9308451893989937</v>
       </c>
       <c r="CL6" t="s">
         <v>115</v>
       </c>
       <c r="CM6" t="n">
-        <v>0.9012858175014593</v>
+        <v>0.9012858175014608</v>
       </c>
       <c r="CN6" t="s">
         <v>116</v>
       </c>
       <c r="CO6" t="n">
-        <v>0.8873513997089583</v>
+        <v>0.8873513997089584</v>
       </c>
       <c r="CP6" t="s">
         <v>116</v>
       </c>
       <c r="CQ6" t="n">
-        <v>0.8605459409356953</v>
+        <v>0.8605459409356946</v>
       </c>
       <c r="CR6" t="s">
         <v>116</v>
       </c>
       <c r="CS6" t="n">
-        <v>0.8929126806105168</v>
+        <v>0.8929126806105159</v>
       </c>
       <c r="CT6" t="s">
         <v>115</v>
       </c>
       <c r="CU6" t="n">
-        <v>0.8836688182987437</v>
+        <v>0.883668818298745</v>
       </c>
       <c r="CV6" t="s">
         <v>116</v>
       </c>
       <c r="CW6" t="n">
-        <v>0.8774840609199828</v>
+        <v>0.8774840609199821</v>
       </c>
       <c r="CX6" t="s">
         <v>116</v>
       </c>
       <c r="CY6" t="n">
-        <v>0.908617981740931</v>
+        <v>0.9086179817409301</v>
       </c>
       <c r="CZ6" t="s">
         <v>116</v>
       </c>
       <c r="DA6" t="n">
-        <v>0.9091467662028792</v>
+        <v>0.909146766202881</v>
       </c>
       <c r="DB6" t="s">
         <v>115</v>
       </c>
       <c r="DC6" t="n">
-        <v>0.849828793461548</v>
+        <v>0.8498287934615474</v>
       </c>
     </row>
   </sheetData>
@@ -8720,7 +8720,7 @@
         <v>112</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="R2" t="s">
         <v>112</v>
@@ -8732,7 +8732,7 @@
         <v>112</v>
       </c>
       <c r="U2" t="n">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="V2" t="s">
         <v>112</v>
@@ -8792,7 +8792,7 @@
         <v>112</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="AP2" t="s">
         <v>112</v>
@@ -8870,7 +8870,7 @@
         <v>112</v>
       </c>
       <c r="BO2" t="n">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BP2" t="s">
         <v>112</v>
@@ -8906,7 +8906,7 @@
         <v>112</v>
       </c>
       <c r="CA2" t="n">
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="CB2" t="s">
         <v>112</v>
@@ -8978,7 +8978,7 @@
         <v>112</v>
       </c>
       <c r="CY2" t="n">
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="CZ2" t="s">
         <v>112</v>
@@ -9001,67 +9001,67 @@
         <v>156</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8182108840439749</v>
+        <v>0.8182108840439738</v>
       </c>
       <c r="D3" t="s">
         <v>157</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9933561858394427</v>
+        <v>0.9933561858394419</v>
       </c>
       <c r="F3" t="s">
         <v>157</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9910485832929381</v>
+        <v>0.9910485832929384</v>
       </c>
       <c r="H3" t="s">
         <v>156</v>
       </c>
       <c r="I3" t="n">
-        <v>0.840787461204807</v>
+        <v>0.8407874612048066</v>
       </c>
       <c r="J3" t="s">
         <v>157</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9538827728171461</v>
+        <v>0.9538827728171453</v>
       </c>
       <c r="L3" t="s">
         <v>157</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9471370489671274</v>
+        <v>0.9471370489671267</v>
       </c>
       <c r="N3" t="s">
         <v>157</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9578645424605191</v>
+        <v>0.9578645424605193</v>
       </c>
       <c r="P3" t="s">
         <v>127</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9869731581246431</v>
+        <v>0.9869731581246429</v>
       </c>
       <c r="R3" t="s">
         <v>156</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8150925452710217</v>
+        <v>0.8150925452710226</v>
       </c>
       <c r="T3" t="s">
         <v>156</v>
       </c>
       <c r="U3" t="n">
-        <v>0.775644165317139</v>
+        <v>0.7756441653171389</v>
       </c>
       <c r="V3" t="s">
         <v>127</v>
       </c>
       <c r="W3" t="n">
-        <v>0.8881285140781363</v>
+        <v>0.8881285140781349</v>
       </c>
       <c r="X3" t="s">
         <v>156</v>
@@ -9073,7 +9073,7 @@
         <v>156</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.7289329706484349</v>
+        <v>0.7289329706484341</v>
       </c>
       <c r="AB3" t="s">
         <v>127</v>
@@ -9085,49 +9085,49 @@
         <v>156</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.7152111768175773</v>
+        <v>0.715211176817577</v>
       </c>
       <c r="AF3" t="s">
         <v>156</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.697935014327881</v>
+        <v>0.6979350143278816</v>
       </c>
       <c r="AH3" t="s">
         <v>156</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.7100833850032561</v>
+        <v>0.7100833850032562</v>
       </c>
       <c r="AJ3" t="s">
         <v>156</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.7271828056694952</v>
+        <v>0.727182805669495</v>
       </c>
       <c r="AL3" t="s">
         <v>156</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.7535125434158199</v>
+        <v>0.75351254341582</v>
       </c>
       <c r="AN3" t="s">
         <v>156</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.7765931177690597</v>
+        <v>0.7765931177690601</v>
       </c>
       <c r="AP3" t="s">
         <v>156</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.7773943427544352</v>
+        <v>0.7773943427544356</v>
       </c>
       <c r="AR3" t="s">
         <v>156</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.7742915151161638</v>
+        <v>0.7742915151161641</v>
       </c>
       <c r="AT3" t="s">
         <v>156</v>
@@ -9151,151 +9151,151 @@
         <v>117</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.7722406149143664</v>
+        <v>0.7722406149143677</v>
       </c>
       <c r="BB3" t="s">
         <v>117</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.7078964426362847</v>
+        <v>0.7078964426362848</v>
       </c>
       <c r="BD3" t="s">
         <v>117</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.7512290579967088</v>
+        <v>0.751229057996709</v>
       </c>
       <c r="BF3" t="s">
         <v>117</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.7176654997831715</v>
+        <v>0.7176654997831703</v>
       </c>
       <c r="BH3" t="s">
         <v>117</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.7350623376317421</v>
+        <v>0.7350623376317414</v>
       </c>
       <c r="BJ3" t="s">
         <v>117</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.8029273681837474</v>
+        <v>0.8029273681837471</v>
       </c>
       <c r="BL3" t="s">
         <v>117</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.9111024328664687</v>
+        <v>0.9111024328664684</v>
       </c>
       <c r="BN3" t="s">
         <v>117</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.8685930162226071</v>
+        <v>0.8685930162226075</v>
       </c>
       <c r="BP3" t="s">
         <v>127</v>
       </c>
       <c r="BQ3" t="n">
-        <v>0.6294936276277623</v>
+        <v>0.6294936276277624</v>
       </c>
       <c r="BR3" t="s">
         <v>117</v>
       </c>
       <c r="BS3" t="n">
-        <v>0.6430168874290643</v>
+        <v>0.6430168874290639</v>
       </c>
       <c r="BT3" t="s">
         <v>156</v>
       </c>
       <c r="BU3" t="n">
-        <v>0.6573220520559175</v>
+        <v>0.6573220520559174</v>
       </c>
       <c r="BV3" t="s">
         <v>156</v>
       </c>
       <c r="BW3" t="n">
-        <v>0.6825944832837757</v>
+        <v>0.6825944832837758</v>
       </c>
       <c r="BX3" t="s">
         <v>156</v>
       </c>
       <c r="BY3" t="n">
-        <v>0.677249929254523</v>
+        <v>0.6772499292545239</v>
       </c>
       <c r="BZ3" t="s">
         <v>127</v>
       </c>
       <c r="CA3" t="n">
-        <v>0.6948561454055977</v>
+        <v>0.694856145405598</v>
       </c>
       <c r="CB3" t="s">
         <v>127</v>
       </c>
       <c r="CC3" t="n">
-        <v>0.6691194046530631</v>
+        <v>0.6691194046530629</v>
       </c>
       <c r="CD3" t="s">
         <v>127</v>
       </c>
       <c r="CE3" t="n">
-        <v>0.6787099398856797</v>
+        <v>0.6787099398856798</v>
       </c>
       <c r="CF3" t="s">
         <v>127</v>
       </c>
       <c r="CG3" t="n">
-        <v>0.676624128118082</v>
+        <v>0.6766241281180828</v>
       </c>
       <c r="CH3" t="s">
         <v>117</v>
       </c>
       <c r="CI3" t="n">
-        <v>0.7468156771964665</v>
+        <v>0.7468156771964661</v>
       </c>
       <c r="CJ3" t="s">
         <v>117</v>
       </c>
       <c r="CK3" t="n">
-        <v>0.7361123301812466</v>
+        <v>0.7361123301812473</v>
       </c>
       <c r="CL3" t="s">
         <v>117</v>
       </c>
       <c r="CM3" t="n">
-        <v>0.7102469777373434</v>
+        <v>0.7102469777373431</v>
       </c>
       <c r="CN3" t="s">
         <v>156</v>
       </c>
       <c r="CO3" t="n">
-        <v>0.6495420556655594</v>
+        <v>0.6495420556655593</v>
       </c>
       <c r="CP3" t="s">
         <v>156</v>
       </c>
       <c r="CQ3" t="n">
-        <v>0.65501679407895</v>
+        <v>0.6550167940789499</v>
       </c>
       <c r="CR3" t="s">
         <v>156</v>
       </c>
       <c r="CS3" t="n">
-        <v>0.6521814107491299</v>
+        <v>0.6521814107491295</v>
       </c>
       <c r="CT3" t="s">
         <v>156</v>
       </c>
       <c r="CU3" t="n">
-        <v>0.6662708363212541</v>
+        <v>0.6662708363212537</v>
       </c>
       <c r="CV3" t="s">
         <v>156</v>
       </c>
       <c r="CW3" t="n">
-        <v>0.6580632362077241</v>
+        <v>0.6580632362077243</v>
       </c>
       <c r="CX3" t="s">
         <v>156</v>
@@ -9307,13 +9307,13 @@
         <v>156</v>
       </c>
       <c r="DA3" t="n">
-        <v>0.6818028100292021</v>
+        <v>0.6818028100292023</v>
       </c>
       <c r="DB3" t="s">
         <v>156</v>
       </c>
       <c r="DC3" t="n">
-        <v>0.6647064484460116</v>
+        <v>0.6647064484460108</v>
       </c>
     </row>
     <row r="4">
@@ -9324,85 +9324,85 @@
         <v>113</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5759800743544232</v>
+        <v>0.5759800743544226</v>
       </c>
       <c r="D4" t="s">
         <v>112</v>
       </c>
       <c r="E4" t="n">
-        <v>0.16229723484734315</v>
+        <v>0.16229723484734257</v>
       </c>
       <c r="F4" t="s">
         <v>112</v>
       </c>
       <c r="G4" t="n">
-        <v>0.19295169790119374</v>
+        <v>0.1929516979011932</v>
       </c>
       <c r="H4" t="s">
         <v>127</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7087863858998136</v>
+        <v>0.7087863858998142</v>
       </c>
       <c r="J4" t="s">
         <v>112</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6852409608791745</v>
+        <v>0.6852409608791804</v>
       </c>
       <c r="L4" t="s">
         <v>112</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7660337408234092</v>
+        <v>0.7660337408234122</v>
       </c>
       <c r="N4" t="s">
         <v>112</v>
       </c>
       <c r="O4" t="n">
-        <v>0.5873400526949895</v>
+        <v>0.5873400526949919</v>
       </c>
       <c r="P4" t="s">
         <v>157</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9076678321166035</v>
+        <v>0.9076678321166025</v>
       </c>
       <c r="R4" t="s">
         <v>127</v>
       </c>
       <c r="S4" t="n">
-        <v>0.5897936093156682</v>
+        <v>0.5897936093156684</v>
       </c>
       <c r="T4" t="s">
         <v>127</v>
       </c>
       <c r="U4" t="n">
-        <v>0.6222799188328457</v>
+        <v>0.6222799188328462</v>
       </c>
       <c r="V4" t="s">
         <v>157</v>
       </c>
       <c r="W4" t="n">
-        <v>0.784078735670731</v>
+        <v>0.7840787356707303</v>
       </c>
       <c r="X4" t="s">
         <v>127</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.7027052300854557</v>
+        <v>0.7027052300854567</v>
       </c>
       <c r="Z4" t="s">
         <v>127</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.6848418917739464</v>
+        <v>0.6848418917739467</v>
       </c>
       <c r="AB4" t="s">
         <v>156</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.7203102095160614</v>
+        <v>0.720310209516062</v>
       </c>
       <c r="AD4" t="s">
         <v>127</v>
@@ -9420,13 +9420,13 @@
         <v>117</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.5832080595963639</v>
+        <v>0.5832080595963655</v>
       </c>
       <c r="AJ4" t="s">
         <v>117</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.5834884599539493</v>
+        <v>0.58348845995395</v>
       </c>
       <c r="AL4" t="s">
         <v>117</v>
@@ -9438,13 +9438,13 @@
         <v>117</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.49028278374273243</v>
+        <v>0.490282783742733</v>
       </c>
       <c r="AP4" t="s">
         <v>117</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.4865172031012461</v>
+        <v>0.48651720310124646</v>
       </c>
       <c r="AR4" t="s">
         <v>117</v>
@@ -9456,37 +9456,37 @@
         <v>117</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.6089454707680593</v>
+        <v>0.6089454707680597</v>
       </c>
       <c r="AV4" t="s">
         <v>117</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.6320676353624354</v>
+        <v>0.6320676353624357</v>
       </c>
       <c r="AX4" t="s">
         <v>117</v>
       </c>
       <c r="AY4" t="n">
-        <v>0.6556526319268663</v>
+        <v>0.655652631926867</v>
       </c>
       <c r="AZ4" t="s">
         <v>156</v>
       </c>
       <c r="BA4" t="n">
-        <v>0.689010699788487</v>
+        <v>0.6890106997884872</v>
       </c>
       <c r="BB4" t="s">
         <v>156</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.6887485359066433</v>
+        <v>0.6887485359066428</v>
       </c>
       <c r="BD4" t="s">
         <v>156</v>
       </c>
       <c r="BE4" t="n">
-        <v>0.6992926242415236</v>
+        <v>0.6992926242415237</v>
       </c>
       <c r="BF4" t="s">
         <v>156</v>
@@ -9498,19 +9498,19 @@
         <v>156</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.674464350074202</v>
+        <v>0.6744643500742017</v>
       </c>
       <c r="BJ4" t="s">
         <v>156</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.6260932752528013</v>
+        <v>0.6260932752528015</v>
       </c>
       <c r="BL4" t="s">
         <v>115</v>
       </c>
       <c r="BM4" t="n">
-        <v>0.666841042119622</v>
+        <v>0.6668410421196216</v>
       </c>
       <c r="BN4" t="s">
         <v>115</v>
@@ -9528,7 +9528,7 @@
         <v>127</v>
       </c>
       <c r="BS4" t="n">
-        <v>0.6408750866539781</v>
+        <v>0.6408750866539775</v>
       </c>
       <c r="BT4" t="s">
         <v>127</v>
@@ -9540,19 +9540,19 @@
         <v>127</v>
       </c>
       <c r="BW4" t="n">
-        <v>0.6376807454068699</v>
+        <v>0.63768074540687</v>
       </c>
       <c r="BX4" t="s">
         <v>127</v>
       </c>
       <c r="BY4" t="n">
-        <v>0.639778163895374</v>
+        <v>0.6397781638953747</v>
       </c>
       <c r="BZ4" t="s">
         <v>156</v>
       </c>
       <c r="CA4" t="n">
-        <v>0.6007893742251407</v>
+        <v>0.600789374225141</v>
       </c>
       <c r="CB4" t="s">
         <v>117</v>
@@ -9564,7 +9564,7 @@
         <v>156</v>
       </c>
       <c r="CE4" t="n">
-        <v>0.6150277139359772</v>
+        <v>0.6150277139359773</v>
       </c>
       <c r="CF4" t="s">
         <v>156</v>
@@ -9576,31 +9576,31 @@
         <v>127</v>
       </c>
       <c r="CI4" t="n">
-        <v>0.6550518761289746</v>
+        <v>0.6550518761289752</v>
       </c>
       <c r="CJ4" t="s">
         <v>127</v>
       </c>
       <c r="CK4" t="n">
-        <v>0.6531918291760532</v>
+        <v>0.653191829176053</v>
       </c>
       <c r="CL4" t="s">
         <v>127</v>
       </c>
       <c r="CM4" t="n">
-        <v>0.6363786755290038</v>
+        <v>0.6363786755290041</v>
       </c>
       <c r="CN4" t="s">
         <v>127</v>
       </c>
       <c r="CO4" t="n">
-        <v>0.6272410336171561</v>
+        <v>0.6272410336171567</v>
       </c>
       <c r="CP4" t="s">
         <v>127</v>
       </c>
       <c r="CQ4" t="n">
-        <v>0.6116811312704781</v>
+        <v>0.6116811312704777</v>
       </c>
       <c r="CR4" t="s">
         <v>127</v>
@@ -9612,25 +9612,25 @@
         <v>127</v>
       </c>
       <c r="CU4" t="n">
-        <v>0.5644740339998645</v>
+        <v>0.5644740339998642</v>
       </c>
       <c r="CV4" t="s">
         <v>127</v>
       </c>
       <c r="CW4" t="n">
-        <v>0.54337131252927</v>
+        <v>0.5433713125292695</v>
       </c>
       <c r="CX4" t="s">
         <v>127</v>
       </c>
       <c r="CY4" t="n">
-        <v>0.4951564803304567</v>
+        <v>0.49515648033045667</v>
       </c>
       <c r="CZ4" t="s">
         <v>127</v>
       </c>
       <c r="DA4" t="n">
-        <v>0.48895580069796574</v>
+        <v>0.48895580069796535</v>
       </c>
       <c r="DB4" t="s">
         <v>127</v>
@@ -9647,175 +9647,175 @@
         <v>146</v>
       </c>
       <c r="C5" t="n">
-        <v>0.24761700304000184</v>
+        <v>0.24761700304000164</v>
       </c>
       <c r="D5" t="s">
         <v>156</v>
       </c>
       <c r="E5" t="n">
-        <v>0.09068362046543874</v>
+        <v>0.09068362046543799</v>
       </c>
       <c r="F5" t="s">
         <v>156</v>
       </c>
       <c r="G5" t="n">
-        <v>0.11649069771069373</v>
+        <v>0.1164906977106935</v>
       </c>
       <c r="H5" t="s">
         <v>157</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6328441718853385</v>
+        <v>0.6328441718853393</v>
       </c>
       <c r="J5" t="s">
         <v>156</v>
       </c>
       <c r="K5" t="n">
-        <v>0.537036136287194</v>
+        <v>0.5370361362871993</v>
       </c>
       <c r="L5" t="s">
         <v>156</v>
       </c>
       <c r="M5" t="n">
-        <v>0.6087364774061652</v>
+        <v>0.6087364774061682</v>
       </c>
       <c r="N5" t="s">
         <v>156</v>
       </c>
       <c r="O5" t="n">
-        <v>0.4448130970015203</v>
+        <v>0.44481309700152216</v>
       </c>
       <c r="P5" t="s">
         <v>156</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.7964724354762039</v>
+        <v>0.7964724354762034</v>
       </c>
       <c r="R5" t="s">
         <v>157</v>
       </c>
       <c r="S5" t="n">
-        <v>0.4920906209814174</v>
+        <v>0.4920906209814178</v>
       </c>
       <c r="T5" t="s">
         <v>157</v>
       </c>
       <c r="U5" t="n">
-        <v>0.504917713100948</v>
+        <v>0.5049177131009488</v>
       </c>
       <c r="V5" t="s">
         <v>156</v>
       </c>
       <c r="W5" t="n">
-        <v>0.7718844630591322</v>
+        <v>0.771884463059132</v>
       </c>
       <c r="X5" t="s">
         <v>157</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.5715043137464805</v>
+        <v>0.5715043137464814</v>
       </c>
       <c r="Z5" t="s">
         <v>157</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.5319899602054189</v>
+        <v>0.5319899602054192</v>
       </c>
       <c r="AB5" t="s">
         <v>157</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.5610867770739086</v>
+        <v>0.5610867770739089</v>
       </c>
       <c r="AD5" t="s">
         <v>117</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.5552222222342479</v>
+        <v>0.5552222222342483</v>
       </c>
       <c r="AF5" t="s">
         <v>117</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.5859848860856435</v>
+        <v>0.5859848860856441</v>
       </c>
       <c r="AH5" t="s">
         <v>127</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.556717699465243</v>
+        <v>0.5567176994652427</v>
       </c>
       <c r="AJ5" t="s">
         <v>127</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.5275085603116512</v>
+        <v>0.5275085603116516</v>
       </c>
       <c r="AL5" t="s">
         <v>127</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.49501761265086874</v>
+        <v>0.4950176126508686</v>
       </c>
       <c r="AN5" t="s">
         <v>127</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.4886400886754992</v>
+        <v>0.4886400886754991</v>
       </c>
       <c r="AP5" t="s">
         <v>127</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0.47357366164363496</v>
+        <v>0.47357366164363507</v>
       </c>
       <c r="AR5" t="s">
         <v>127</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.48083293572108016</v>
+        <v>0.4808329357210806</v>
       </c>
       <c r="AT5" t="s">
         <v>127</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.5334232888785638</v>
+        <v>0.5334232888785636</v>
       </c>
       <c r="AV5" t="s">
         <v>127</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.5170266239894737</v>
+        <v>0.5170266239894735</v>
       </c>
       <c r="AX5" t="s">
         <v>127</v>
       </c>
       <c r="AY5" t="n">
-        <v>0.5267852299646214</v>
+        <v>0.5267852299646217</v>
       </c>
       <c r="AZ5" t="s">
         <v>115</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.5340412752519136</v>
+        <v>0.5340412752519142</v>
       </c>
       <c r="BB5" t="s">
         <v>127</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.5549044918266584</v>
+        <v>0.5549044918266574</v>
       </c>
       <c r="BD5" t="s">
         <v>115</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.536325921875024</v>
+        <v>0.5363259218750248</v>
       </c>
       <c r="BF5" t="s">
         <v>127</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.544180210303288</v>
+        <v>0.5441802103032882</v>
       </c>
       <c r="BH5" t="s">
         <v>127</v>
@@ -9827,25 +9827,25 @@
         <v>115</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.575526513613856</v>
+        <v>0.5755265136138554</v>
       </c>
       <c r="BL5" t="s">
         <v>156</v>
       </c>
       <c r="BM5" t="n">
-        <v>0.5958603256984952</v>
+        <v>0.595860325698495</v>
       </c>
       <c r="BN5" t="s">
         <v>127</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.5907591635912913</v>
+        <v>0.5907591635912908</v>
       </c>
       <c r="BP5" t="s">
         <v>117</v>
       </c>
       <c r="BQ5" t="n">
-        <v>0.5911029467463877</v>
+        <v>0.591102946746387</v>
       </c>
       <c r="BR5" t="s">
         <v>156</v>
@@ -9857,109 +9857,109 @@
         <v>117</v>
       </c>
       <c r="BU5" t="n">
-        <v>0.525471192470393</v>
+        <v>0.5254711924703936</v>
       </c>
       <c r="BV5" t="s">
         <v>117</v>
       </c>
       <c r="BW5" t="n">
-        <v>0.3998810908213701</v>
+        <v>0.3998810908213702</v>
       </c>
       <c r="BX5" t="s">
         <v>117</v>
       </c>
       <c r="BY5" t="n">
-        <v>0.42904237434080983</v>
+        <v>0.42904237434080966</v>
       </c>
       <c r="BZ5" t="s">
         <v>117</v>
       </c>
       <c r="CA5" t="n">
-        <v>0.5708635072157175</v>
+        <v>0.5708635072157172</v>
       </c>
       <c r="CB5" t="s">
         <v>156</v>
       </c>
       <c r="CC5" t="n">
-        <v>0.6039734576684271</v>
+        <v>0.603973457668427</v>
       </c>
       <c r="CD5" t="s">
         <v>117</v>
       </c>
       <c r="CE5" t="n">
-        <v>0.6084031145851869</v>
+        <v>0.6084031145851867</v>
       </c>
       <c r="CF5" t="s">
         <v>117</v>
       </c>
       <c r="CG5" t="n">
-        <v>0.5843482150510948</v>
+        <v>0.5843482150510952</v>
       </c>
       <c r="CH5" t="s">
         <v>156</v>
       </c>
       <c r="CI5" t="n">
-        <v>0.5959899151152653</v>
+        <v>0.5959899151152658</v>
       </c>
       <c r="CJ5" t="s">
         <v>156</v>
       </c>
       <c r="CK5" t="n">
-        <v>0.5958743043590147</v>
+        <v>0.5958743043590148</v>
       </c>
       <c r="CL5" t="s">
         <v>156</v>
       </c>
       <c r="CM5" t="n">
-        <v>0.6018449336434736</v>
+        <v>0.6018449336434735</v>
       </c>
       <c r="CN5" t="s">
         <v>117</v>
       </c>
       <c r="CO5" t="n">
-        <v>0.46509003238435914</v>
+        <v>0.46509003238435925</v>
       </c>
       <c r="CP5" t="s">
         <v>117</v>
       </c>
       <c r="CQ5" t="n">
-        <v>0.45644852506623335</v>
+        <v>0.4564485250662334</v>
       </c>
       <c r="CR5" t="s">
         <v>117</v>
       </c>
       <c r="CS5" t="n">
-        <v>0.5188076168501068</v>
+        <v>0.5188076168501077</v>
       </c>
       <c r="CT5" t="s">
         <v>117</v>
       </c>
       <c r="CU5" t="n">
-        <v>0.4751908105349651</v>
+        <v>0.4751908105349648</v>
       </c>
       <c r="CV5" t="s">
         <v>117</v>
       </c>
       <c r="CW5" t="n">
-        <v>0.3911501689173783</v>
+        <v>0.391150168917378</v>
       </c>
       <c r="CX5" t="s">
         <v>117</v>
       </c>
       <c r="CY5" t="n">
-        <v>0.41971052780047197</v>
+        <v>0.41971052780047235</v>
       </c>
       <c r="CZ5" t="s">
         <v>158</v>
       </c>
       <c r="DA5" t="n">
-        <v>0.37656343827874367</v>
+        <v>0.37656343827874406</v>
       </c>
       <c r="DB5" t="s">
         <v>158</v>
       </c>
       <c r="DC5" t="n">
-        <v>0.40500636443912325</v>
+        <v>0.40500636443912275</v>
       </c>
     </row>
     <row r="6">
@@ -9970,61 +9970,61 @@
         <v>115</v>
       </c>
       <c r="C6" t="n">
-        <v>0.22610091408686644</v>
+        <v>0.22610091408686642</v>
       </c>
       <c r="D6" t="s">
         <v>113</v>
       </c>
       <c r="E6" t="n">
-        <v>0.05331446714231956</v>
+        <v>0.05331446714231952</v>
       </c>
       <c r="F6" t="s">
         <v>113</v>
       </c>
       <c r="G6" t="n">
-        <v>0.058388307967347904</v>
+        <v>0.05838830796734807</v>
       </c>
       <c r="H6" t="s">
         <v>113</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3632623458819715</v>
+        <v>0.36326234588197215</v>
       </c>
       <c r="J6" t="s">
         <v>113</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2819081560001142</v>
+        <v>0.2819081560001173</v>
       </c>
       <c r="L6" t="s">
         <v>113</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2958604493580801</v>
+        <v>0.29586044935808187</v>
       </c>
       <c r="N6" t="s">
         <v>113</v>
       </c>
       <c r="O6" t="n">
-        <v>0.22378731744549787</v>
+        <v>0.22378731744549815</v>
       </c>
       <c r="P6" t="s">
         <v>113</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.4338220461826129</v>
+        <v>0.43382204618261316</v>
       </c>
       <c r="R6" t="s">
         <v>113</v>
       </c>
       <c r="S6" t="n">
-        <v>0.4125337691484259</v>
+        <v>0.4125337691484257</v>
       </c>
       <c r="T6" t="s">
         <v>113</v>
       </c>
       <c r="U6" t="n">
-        <v>0.4151628757260696</v>
+        <v>0.41516287572606986</v>
       </c>
       <c r="V6" t="s">
         <v>113</v>
@@ -10036,79 +10036,79 @@
         <v>113</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.46559971839486913</v>
+        <v>0.46559971839487</v>
       </c>
       <c r="Z6" t="s">
         <v>113</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.5062426335517064</v>
+        <v>0.506242633551706</v>
       </c>
       <c r="AB6" t="s">
         <v>117</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.5080937705069868</v>
+        <v>0.5080937705069878</v>
       </c>
       <c r="AD6" t="s">
         <v>157</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.47907489162381317</v>
+        <v>0.4790748916238131</v>
       </c>
       <c r="AF6" t="s">
         <v>113</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.4860066889383533</v>
+        <v>0.4860066889383534</v>
       </c>
       <c r="AH6" t="s">
         <v>113</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.49349298869642877</v>
+        <v>0.49349298869642866</v>
       </c>
       <c r="AJ6" t="s">
         <v>113</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.46645710258480805</v>
+        <v>0.4664571025848081</v>
       </c>
       <c r="AL6" t="s">
         <v>113</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.43028853065865785</v>
+        <v>0.4302885306586579</v>
       </c>
       <c r="AN6" t="s">
         <v>113</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.4081129703295772</v>
+        <v>0.40811297032957716</v>
       </c>
       <c r="AP6" t="s">
         <v>113</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.3866592703577748</v>
+        <v>0.3866592703577744</v>
       </c>
       <c r="AR6" t="s">
         <v>113</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.3630495215159079</v>
+        <v>0.36304952151590875</v>
       </c>
       <c r="AT6" t="s">
         <v>115</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.38575739059801484</v>
+        <v>0.3857573905980148</v>
       </c>
       <c r="AV6" t="s">
         <v>115</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.39931666180315323</v>
+        <v>0.3993166618031533</v>
       </c>
       <c r="AX6" t="s">
         <v>115</v>
@@ -10120,37 +10120,37 @@
         <v>127</v>
       </c>
       <c r="BA6" t="n">
-        <v>0.5337431174993315</v>
+        <v>0.5337431174993318</v>
       </c>
       <c r="BB6" t="s">
         <v>115</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.4919463468504365</v>
+        <v>0.4919463468504358</v>
       </c>
       <c r="BD6" t="s">
         <v>127</v>
       </c>
       <c r="BE6" t="n">
-        <v>0.5190315506348026</v>
+        <v>0.5190315506348028</v>
       </c>
       <c r="BF6" t="s">
         <v>115</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.5250214363632919</v>
+        <v>0.5250214363632907</v>
       </c>
       <c r="BH6" t="s">
         <v>115</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.5227156857442228</v>
+        <v>0.5227156857442233</v>
       </c>
       <c r="BJ6" t="s">
         <v>127</v>
       </c>
       <c r="BK6" t="n">
-        <v>0.5721746567003542</v>
+        <v>0.5721746567003536</v>
       </c>
       <c r="BL6" t="s">
         <v>114</v>
@@ -10162,61 +10162,61 @@
         <v>156</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.5639817637220133</v>
+        <v>0.5639817637220134</v>
       </c>
       <c r="BP6" t="s">
         <v>115</v>
       </c>
       <c r="BQ6" t="n">
-        <v>0.44703933596231654</v>
+        <v>0.44703933596231565</v>
       </c>
       <c r="BR6" t="s">
         <v>115</v>
       </c>
       <c r="BS6" t="n">
-        <v>0.478347048987711</v>
+        <v>0.4783470489877102</v>
       </c>
       <c r="BT6" t="s">
         <v>113</v>
       </c>
       <c r="BU6" t="n">
-        <v>0.39543066574777597</v>
+        <v>0.39543066574777586</v>
       </c>
       <c r="BV6" t="s">
         <v>113</v>
       </c>
       <c r="BW6" t="n">
-        <v>0.3167081045781994</v>
+        <v>0.3167081045781997</v>
       </c>
       <c r="BX6" t="s">
         <v>113</v>
       </c>
       <c r="BY6" t="n">
-        <v>0.3272604599630147</v>
+        <v>0.32726045996301556</v>
       </c>
       <c r="BZ6" t="s">
         <v>115</v>
       </c>
       <c r="CA6" t="n">
-        <v>0.3699296251921518</v>
+        <v>0.36992962519215206</v>
       </c>
       <c r="CB6" t="s">
         <v>115</v>
       </c>
       <c r="CC6" t="n">
-        <v>0.43605584943105374</v>
+        <v>0.4360558494310536</v>
       </c>
       <c r="CD6" t="s">
         <v>115</v>
       </c>
       <c r="CE6" t="n">
-        <v>0.42838067415540426</v>
+        <v>0.4283806741554043</v>
       </c>
       <c r="CF6" t="s">
         <v>113</v>
       </c>
       <c r="CG6" t="n">
-        <v>0.41676175824618966</v>
+        <v>0.4167617582461894</v>
       </c>
       <c r="CH6" t="s">
         <v>115</v>
@@ -10228,61 +10228,61 @@
         <v>115</v>
       </c>
       <c r="CK6" t="n">
-        <v>0.5334910386645297</v>
+        <v>0.5334910386645303</v>
       </c>
       <c r="CL6" t="s">
         <v>115</v>
       </c>
       <c r="CM6" t="n">
-        <v>0.5173409600526162</v>
+        <v>0.5173409600526166</v>
       </c>
       <c r="CN6" t="s">
         <v>113</v>
       </c>
       <c r="CO6" t="n">
-        <v>0.3387445209943942</v>
+        <v>0.3387445209943937</v>
       </c>
       <c r="CP6" t="s">
         <v>113</v>
       </c>
       <c r="CQ6" t="n">
-        <v>0.3310830365050641</v>
+        <v>0.3310830365050642</v>
       </c>
       <c r="CR6" t="s">
         <v>113</v>
       </c>
       <c r="CS6" t="n">
-        <v>0.35413889785244623</v>
+        <v>0.3541388978524461</v>
       </c>
       <c r="CT6" t="s">
         <v>113</v>
       </c>
       <c r="CU6" t="n">
-        <v>0.3429920559920857</v>
+        <v>0.3429920559920855</v>
       </c>
       <c r="CV6" t="s">
         <v>128</v>
       </c>
       <c r="CW6" t="n">
-        <v>0.38004277494262706</v>
+        <v>0.38004277494262695</v>
       </c>
       <c r="CX6" t="s">
         <v>128</v>
       </c>
       <c r="CY6" t="n">
-        <v>0.35372543299277953</v>
+        <v>0.35372543299277964</v>
       </c>
       <c r="CZ6" t="s">
         <v>128</v>
       </c>
       <c r="DA6" t="n">
-        <v>0.3400792668616443</v>
+        <v>0.34007926686164436</v>
       </c>
       <c r="DB6" t="s">
         <v>128</v>
       </c>
       <c r="DC6" t="n">
-        <v>0.3587332949753233</v>
+        <v>0.35873329497532275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>